<commit_message>
Well Completion G Well_No field int -> str
</commit_message>
<xml_diff>
--- a/src/ogrre_data_cleaning/processor_schemas/ISGS Well Completion Schema.xlsx
+++ b/src/ogrre_data_cleaning/processor_schemas/ISGS Well Completion Schema.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6502" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6501" uniqueCount="871">
   <si>
     <t>Naming Scheme as of 6/17/2024</t>
   </si>
@@ -3986,7 +3986,7 @@
     <xdr:ext cx="2028825" cy="2762250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are 4 minor variations of this format" id="0" name="image6.png" title="Completion_A"/>
+        <xdr:cNvPr descr="There are 4 minor variations of this format" id="0" name="image3.png" title="Completion_A"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4042,7 +4042,7 @@
     <xdr:ext cx="2000250" cy="2752725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Completion_C Page 2"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Completion_C Page 2"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4070,7 +4070,7 @@
     <xdr:ext cx="1981200" cy="2705100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are two minor variations of this format" id="0" name="image3.png" title="Competion_D Page 1"/>
+        <xdr:cNvPr descr="There are two minor variations of this format" id="0" name="image9.png" title="Competion_D Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4098,7 +4098,7 @@
     <xdr:ext cx="1990725" cy="2705100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="There are two variations of this format" id="0" name="image5.png" title="Completion_D Page 2"/>
+        <xdr:cNvPr descr="There are two variations of this format" id="0" name="image1.png" title="Completion_D Page 2"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4126,7 +4126,7 @@
     <xdr:ext cx="2047875" cy="2781300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Completion_E Page 1"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Completion_E Page 1"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4154,7 +4154,7 @@
     <xdr:ext cx="1952625" cy="2781300"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Completion_E"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Completion_E"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4182,7 +4182,7 @@
     <xdr:ext cx="1762125" cy="2324100"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4210,7 +4210,7 @@
     <xdr:ext cx="2581275" cy="2133600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -14095,11 +14095,9 @@
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="26" t="s">
-        <v>441</v>
-      </c>
-      <c r="I6" s="26" t="s">
-        <v>442</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="I6" s="26"/>
       <c r="J6" s="26"/>
       <c r="K6" s="26"/>
       <c r="L6" s="26" t="s">

</xml_diff>